<commit_message>
refactored formatted strings in final report
</commit_message>
<xml_diff>
--- a/data/cashflow-2022.xlsx
+++ b/data/cashflow-2022.xlsx
@@ -16,17 +16,17 @@
     <definedName name="Entertainment">Lists!$G$2:$G$5</definedName>
     <definedName name="ShoppingList">Lists!$B$2:$B$5</definedName>
     <definedName name="CareerList">Lists!$H$2:$H$4</definedName>
-    <definedName hidden="1" localSheetId="0" name="Z_7D6E590C_26E8_41FD_8B99_D96F3E596134_.wvu.FilterData">'Data '!$A$1:$G$991</definedName>
+    <definedName hidden="1" localSheetId="0" name="Z_573DC077_1E55_4020_80A8_E5CF875F7882_.wvu.FilterData">'Data '!$A$1:$G$991</definedName>
   </definedNames>
   <calcPr/>
   <customWorkbookViews>
-    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{7D6E590C-26E8-41FD-8B99-D96F3E596134}" name="Filter 1"/>
+    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{573DC077-1E55-4020-80A8-E5CF875F7882}" name="Filter 1"/>
   </customWorkbookViews>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1793" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1805" uniqueCount="252">
   <si>
     <t>Type</t>
   </si>
@@ -10002,68 +10002,106 @@
         <v>7</v>
       </c>
       <c r="B411" s="7" t="s">
-        <v>147</v>
+        <v>38</v>
       </c>
       <c r="C411" s="9">
-        <v>51.86</v>
+        <v>33.9</v>
       </c>
       <c r="D411" s="6">
-        <v>44926.0</v>
+        <v>44924.0</v>
       </c>
       <c r="E411" s="7" t="s">
-        <v>107</v>
+        <v>39</v>
       </c>
       <c r="F411" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="G411" s="8" t="s">
-        <v>241</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="G411" s="19"/>
     </row>
     <row r="412">
       <c r="A412" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B412" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="C412" s="9"/>
+        <v>147</v>
+      </c>
+      <c r="C412" s="9">
+        <v>51.86</v>
+      </c>
       <c r="D412" s="6">
         <v>44926.0</v>
       </c>
       <c r="E412" s="7" t="s">
-        <v>9</v>
+        <v>107</v>
       </c>
       <c r="F412" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="G412" s="8" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="413">
+      <c r="A413" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B413" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C413" s="9">
+        <v>38.77</v>
+      </c>
+      <c r="D413" s="6">
+        <v>44926.0</v>
+      </c>
+      <c r="E413" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F413" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="G412" s="19"/>
-    </row>
-    <row r="413">
-      <c r="A413" s="24"/>
-      <c r="B413" s="7"/>
-      <c r="C413" s="9"/>
-      <c r="D413" s="6"/>
-      <c r="E413" s="7"/>
-      <c r="F413" s="7"/>
       <c r="G413" s="19"/>
     </row>
     <row r="414">
-      <c r="A414" s="24"/>
-      <c r="B414" s="7"/>
-      <c r="C414" s="9"/>
-      <c r="D414" s="6"/>
-      <c r="E414" s="7"/>
-      <c r="F414" s="7"/>
+      <c r="A414" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B414" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="C414" s="9">
+        <v>51.96</v>
+      </c>
+      <c r="D414" s="6">
+        <v>44926.0</v>
+      </c>
+      <c r="E414" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F414" s="7" t="s">
+        <v>10</v>
+      </c>
       <c r="G414" s="19"/>
     </row>
     <row r="415">
-      <c r="A415" s="24"/>
-      <c r="B415" s="7"/>
-      <c r="C415" s="9"/>
-      <c r="D415" s="6"/>
-      <c r="E415" s="7"/>
-      <c r="F415" s="7"/>
+      <c r="A415" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B415" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C415" s="9">
+        <v>2.31</v>
+      </c>
+      <c r="D415" s="6">
+        <v>44926.0</v>
+      </c>
+      <c r="E415" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F415" s="7" t="s">
+        <v>10</v>
+      </c>
       <c r="G415" s="19"/>
     </row>
     <row r="416">
@@ -15252,7 +15290,7 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{7D6E590C-26E8-41FD-8B99-D96F3E596134}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{573DC077-1E55-4020-80A8-E5CF875F7882}" filter="1" showAutoFilter="1">
       <autoFilter ref="$A$1:$G$991"/>
     </customSheetView>
   </customSheetViews>

</xml_diff>